<commit_message>
update impact factors and improve import routine
</commit_message>
<xml_diff>
--- a/impactFactors/distributable/availableMaterialsAndDispositions.xlsx
+++ b/impactFactors/distributable/availableMaterialsAndDispositions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13128" windowHeight="6108"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>material</t>
   </si>
@@ -51,10 +51,16 @@
     <t>recyclingToAggregate</t>
   </si>
   <si>
+    <t>recyclingToContainer &lt;LC&gt;</t>
+  </si>
+  <si>
+    <t>recyclingToFiberglass</t>
+  </si>
+  <si>
+    <t>reuseContainer</t>
+  </si>
+  <si>
     <t>recyclingToContainer</t>
-  </si>
-  <si>
-    <t>recyclingToFiberglass</t>
   </si>
   <si>
     <t>AcceptedOtherSteel</t>
@@ -197,7 +203,7 @@
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment textRotation="90"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -495,29 +501,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:L33"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
-    <col min="2" max="2" width="8.21875" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="8.21875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
-    <col min="6" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="8.77734375" customWidth="1"/>
-    <col min="9" max="9" width="7.5546875" customWidth="1"/>
-    <col min="10" max="10" width="6.88671875" customWidth="1"/>
-    <col min="11" max="11" width="7.77734375" customWidth="1"/>
-    <col min="12" max="12" width="8.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="104.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,10 +549,16 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -572,9 +573,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -589,9 +590,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
@@ -606,9 +607,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -626,9 +627,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -646,9 +647,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -666,9 +667,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -680,9 +681,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" t="b">
         <v>1</v>
@@ -697,9 +698,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -720,9 +721,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -737,9 +738,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -754,9 +755,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -779,10 +780,16 @@
       <c r="L13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -797,9 +804,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
@@ -814,9 +821,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C16" t="b">
         <v>1</v>
@@ -831,9 +838,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -848,9 +855,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
@@ -865,9 +872,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -902,10 +909,16 @@
       <c r="L19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M19" t="b">
+        <v>1</v>
+      </c>
+      <c r="N19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -920,9 +933,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -940,9 +953,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -957,9 +970,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B23" t="b">
         <v>1</v>
@@ -977,9 +990,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
@@ -997,9 +1010,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C25" t="b">
         <v>1</v>
@@ -1014,9 +1027,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C26" t="b">
         <v>1</v>
@@ -1031,9 +1044,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C27" t="b">
         <v>1</v>
@@ -1048,9 +1061,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B28" t="b">
         <v>1</v>
@@ -1068,9 +1081,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
@@ -1085,9 +1098,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B30" t="b">
         <v>1</v>
@@ -1105,9 +1118,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
@@ -1122,9 +1135,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C32" t="b">
         <v>1</v>
@@ -1139,9 +1152,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B33" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
import factors from GaBi export 20210831
</commit_message>
<xml_diff>
--- a/impactFactors/distributable/availableMaterialsAndDispositions.xlsx
+++ b/impactFactors/distributable/availableMaterialsAndDispositions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t xml:space="preserve">material</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t xml:space="preserve">reuseContainer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reuseGeneric</t>
   </si>
   <si>
     <t xml:space="preserve">AcceptedOtherSteel</t>
@@ -518,10 +521,13 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -543,10 +549,11 @@
       <c r="K2"/>
       <c r="L2"/>
       <c r="M2"/>
+      <c r="N2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -568,10 +575,11 @@
       <c r="K3"/>
       <c r="L3"/>
       <c r="M3"/>
+      <c r="N3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4"/>
       <c r="C4" t="b">
@@ -593,10 +601,11 @@
       <c r="K4"/>
       <c r="L4"/>
       <c r="M4"/>
+      <c r="N4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -620,10 +629,11 @@
       <c r="K5"/>
       <c r="L5"/>
       <c r="M5"/>
+      <c r="N5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -647,10 +657,11 @@
       <c r="K6"/>
       <c r="L6"/>
       <c r="M6"/>
+      <c r="N6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -674,10 +685,11 @@
       <c r="K7"/>
       <c r="L7"/>
       <c r="M7"/>
+      <c r="N7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8"/>
       <c r="C8" t="b">
@@ -697,10 +709,11 @@
       <c r="K8"/>
       <c r="L8"/>
       <c r="M8"/>
+      <c r="N8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9"/>
       <c r="C9" t="b">
@@ -722,10 +735,11 @@
       <c r="K9"/>
       <c r="L9"/>
       <c r="M9"/>
+      <c r="N9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -751,10 +765,11 @@
       <c r="K10"/>
       <c r="L10"/>
       <c r="M10"/>
+      <c r="N10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11"/>
       <c r="C11" t="b">
@@ -776,10 +791,11 @@
       <c r="K11"/>
       <c r="L11"/>
       <c r="M11"/>
+      <c r="N11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12"/>
       <c r="C12" t="b">
@@ -801,10 +817,11 @@
       <c r="K12"/>
       <c r="L12"/>
       <c r="M12"/>
+      <c r="N12"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -834,10 +851,11 @@
       <c r="M13" t="b">
         <v>1</v>
       </c>
+      <c r="N13"/>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -859,10 +877,11 @@
       <c r="K14"/>
       <c r="L14"/>
       <c r="M14"/>
+      <c r="N14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B15"/>
       <c r="C15" t="b">
@@ -884,10 +903,11 @@
       <c r="K15"/>
       <c r="L15"/>
       <c r="M15"/>
+      <c r="N15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16"/>
       <c r="C16" t="b">
@@ -909,10 +929,11 @@
       <c r="K16"/>
       <c r="L16"/>
       <c r="M16"/>
+      <c r="N16"/>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17"/>
       <c r="C17" t="b">
@@ -934,10 +955,11 @@
       <c r="K17"/>
       <c r="L17"/>
       <c r="M17"/>
+      <c r="N17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
@@ -959,10 +981,11 @@
       <c r="K18"/>
       <c r="L18"/>
       <c r="M18"/>
+      <c r="N18"/>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -986,10 +1009,11 @@
       <c r="K19"/>
       <c r="L19"/>
       <c r="M19"/>
+      <c r="N19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B20"/>
       <c r="C20" t="b">
@@ -1011,10 +1035,11 @@
       <c r="K20"/>
       <c r="L20"/>
       <c r="M20"/>
+      <c r="N20"/>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -1038,10 +1063,11 @@
       <c r="K21"/>
       <c r="L21"/>
       <c r="M21"/>
+      <c r="N21"/>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B22"/>
       <c r="C22" t="b">
@@ -1063,10 +1089,11 @@
       <c r="K22"/>
       <c r="L22"/>
       <c r="M22"/>
+      <c r="N22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B23" t="b">
         <v>1</v>
@@ -1090,10 +1117,11 @@
       <c r="K23"/>
       <c r="L23"/>
       <c r="M23"/>
+      <c r="N23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
@@ -1117,10 +1145,11 @@
       <c r="K24"/>
       <c r="L24"/>
       <c r="M24"/>
+      <c r="N24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B25"/>
       <c r="C25" t="b">
@@ -1142,10 +1171,11 @@
       <c r="K25"/>
       <c r="L25"/>
       <c r="M25"/>
+      <c r="N25"/>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26"/>
       <c r="C26" t="b">
@@ -1167,10 +1197,11 @@
       <c r="K26"/>
       <c r="L26"/>
       <c r="M26"/>
+      <c r="N26"/>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B27"/>
       <c r="C27" t="b">
@@ -1192,10 +1223,11 @@
       <c r="K27"/>
       <c r="L27"/>
       <c r="M27"/>
+      <c r="N27"/>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B28" t="b">
         <v>1</v>
@@ -1219,10 +1251,11 @@
       <c r="K28"/>
       <c r="L28"/>
       <c r="M28"/>
+      <c r="N28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
@@ -1244,10 +1277,11 @@
       <c r="K29"/>
       <c r="L29"/>
       <c r="M29"/>
+      <c r="N29"/>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B30" t="b">
         <v>1</v>
@@ -1271,10 +1305,11 @@
       <c r="K30"/>
       <c r="L30"/>
       <c r="M30"/>
+      <c r="N30"/>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
@@ -1296,10 +1331,11 @@
       <c r="K31"/>
       <c r="L31"/>
       <c r="M31"/>
+      <c r="N31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B32"/>
       <c r="C32" t="b">
@@ -1321,10 +1357,13 @@
       <c r="K32"/>
       <c r="L32"/>
       <c r="M32"/>
+      <c r="N32" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B33" t="b">
         <v>1</v>
@@ -1350,6 +1389,7 @@
       <c r="K33"/>
       <c r="L33"/>
       <c r="M33"/>
+      <c r="N33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
import factors from 2022 and revise treatment of the Other material category
</commit_message>
<xml_diff>
--- a/impactFactors/distributable/availableMaterialsAndDispositions.xlsx
+++ b/impactFactors/distributable/availableMaterialsAndDispositions.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -474,10 +474,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>

</xml_diff>